<commit_message>
end of 4th week
</commit_message>
<xml_diff>
--- a/2_Week4. Algorithms formalization/Resume2_4.xlsx
+++ b/2_Week4. Algorithms formalization/Resume2_4.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Фамилия</t>
   </si>
@@ -107,6 +107,15 @@
   </si>
   <si>
     <t>Руссификация приложения</t>
+  </si>
+  <si>
+    <t>5-</t>
+  </si>
+  <si>
+    <t>4-</t>
+  </si>
+  <si>
+    <t>позже</t>
   </si>
 </sst>
 </file>
@@ -463,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,7 +516,9 @@
       <c r="C2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="4">
+        <v>0.5</v>
+      </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
@@ -522,7 +533,9 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
@@ -537,7 +550,9 @@
       <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="4"/>
+      <c r="D4" s="4">
+        <v>0.9</v>
+      </c>
       <c r="E4" s="2" t="s">
         <v>6</v>
       </c>
@@ -552,7 +567,9 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
@@ -567,7 +584,9 @@
       <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="4"/>
+      <c r="D6" s="4">
+        <v>0.8</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
       </c>
@@ -582,7 +601,9 @@
       <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4">
+        <v>0.7</v>
+      </c>
       <c r="E7" s="2" t="s">
         <v>8</v>
       </c>
@@ -597,7 +618,9 @@
       <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -609,7 +632,9 @@
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
@@ -621,7 +646,9 @@
       <c r="C10" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
@@ -631,7 +658,9 @@
       <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
@@ -651,21 +680,27 @@
       <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>4</v>
+      </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>5</v>
+      </c>
       <c r="C16"/>
       <c r="D16" s="4"/>
     </row>
@@ -673,38 +708,50 @@
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">

</xml_diff>

<commit_message>
updated marks for 4th week
</commit_message>
<xml_diff>
--- a/2_Week4. Algorithms formalization/Resume2_4.xlsx
+++ b/2_Week4. Algorithms formalization/Resume2_4.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t>Фамилия</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>4-</t>
-  </si>
-  <si>
-    <t>позже</t>
   </si>
 </sst>
 </file>
@@ -472,8 +469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +514,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="4">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -708,8 +705,8 @@
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>33</v>
+      <c r="B17" s="2">
+        <v>2</v>
       </c>
       <c r="D17" s="4"/>
     </row>
@@ -726,7 +723,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>